<commit_message>
Added showing product image functionality in a modal
</commit_message>
<xml_diff>
--- a/server/uploads/priceList.xlsx
+++ b/server/uploads/priceList.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="99">
   <si>
     <t xml:space="preserve">cod</t>
   </si>
@@ -31,166 +31,292 @@
     <t xml:space="preserve">price</t>
   </si>
   <si>
-    <t xml:space="preserve">038162</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BUJE REDUCCION HrBr 13 x 9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">038163</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BUJE REDUCCION HrBr 25 x 19</t>
-  </si>
-  <si>
-    <t xml:space="preserve">038164</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CODO NORMAL HrBr 9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">038165</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CODO NORMAL HrBr 13</t>
-  </si>
-  <si>
-    <t xml:space="preserve">038166</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CODO NORMAL HrBr 19</t>
-  </si>
-  <si>
-    <t xml:space="preserve">038167</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CODO NORMAL HrBr 25</t>
-  </si>
-  <si>
-    <t xml:space="preserve">038168</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CODO REDUCCION HrBr 9 x RH 1/2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">038169</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CODO REDUCCION HrBr 13 x RH 3/8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">038170</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CODO REDUCCION HrBr 13 x RH 3/4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">038171</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CODO REDUCCION HrBr 19 x RH 1/2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">038172</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CODO HrBr 13 x RH 1/2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">038173</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CODO HrBr 19 x RH 3/4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">038174</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CODO HrBr 25 x RH 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">038175</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CODO HrBr 13 x RM 1/2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">038176</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CODO HrBr 19 x RM 3/4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">038177</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CODO HrBr 25 x RM 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">038178</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CURVA HrBr 13 A 45</t>
-  </si>
-  <si>
-    <t xml:space="preserve">038179</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CURVA HrBr 19 A 45</t>
-  </si>
-  <si>
-    <t xml:space="preserve">038181</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CURVA HrBr 25 A 45</t>
-  </si>
-  <si>
-    <t xml:space="preserve">038182</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CURVA HrBr 13 A 90</t>
-  </si>
-  <si>
-    <t xml:space="preserve">038183</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CURVA HrBr 19 A 90</t>
-  </si>
-  <si>
-    <t xml:space="preserve">450495</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CURVA HrBr 25 A 90</t>
-  </si>
-  <si>
-    <t xml:space="preserve">450549</t>
-  </si>
-  <si>
-    <t xml:space="preserve">REDUCCION HrBr 19 x 13</t>
-  </si>
-  <si>
-    <t xml:space="preserve">450550</t>
-  </si>
-  <si>
-    <t xml:space="preserve">REDUCCION HrBr 25 x 19</t>
-  </si>
-  <si>
-    <t xml:space="preserve">450597</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TEE NORMAL HrBr 9 x 9 x 9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">450598</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TEE NORMAL HrBr 13 x 13 x 13</t>
-  </si>
-  <si>
-    <t xml:space="preserve">450599</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TEE NORMAL HrBr 19 x 19 x 19</t>
+    <t xml:space="preserve">002005</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ABRAZADERA CREMALLERA  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">004019</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ABRAZADERA 2032 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">008053</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CODO GALVA HM 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">018003</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CODO BRONCE GAS HH 1/4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">022049</t>
+  </si>
+  <si>
+    <t xml:space="preserve">REDUCCION BRONCE GAS MM </t>
+  </si>
+  <si>
+    <t xml:space="preserve">024049</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CODO PPN HH 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">024085</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CUPLA PPN 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">032105</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TEE NORMAL 63 x 50 x 63 AS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">038130</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CUPLA REDUCCION 32 X 25  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">038189</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UNION DOBLE MIXTA M 32 X 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">040127</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ESPIGA PPL 3/4 x RM 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">042039</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TAPA SIGAS 20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">054025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ARANDELA FIBRA N22 1 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">090055</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CABEZAL LPIAZZA LLAVE PASO 3/4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">132015</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CAÑO MAGNUM PN20 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">192017</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CANILLA PICO MANGA 1  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">192029</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LLAVE ESFERICA   3/4 PVC DUKE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">192044</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VALVULA EVOLUTION 3/4 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">192059</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SOPAPA 1 1/4 / 40MM  PVC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">198011</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CAMARA INSA M 1/2 PVC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">198023</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CHAVETA ROSCADA x 100</t>
+  </si>
+  <si>
+    <t xml:space="preserve">202049</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FERRUM BIDET 1 AGUJERO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">202458</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FERRUM BARRAL FIJO 50cm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">246019</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LLAVE GAS 2 ALARSA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">246051</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LLAVE GAS   3/4 GAS </t>
+  </si>
+  <si>
+    <t xml:space="preserve">262004</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LLAVE SIGAS ESFERICA 32</t>
+  </si>
+  <si>
+    <t xml:space="preserve">270021</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MEDIA UNION REDUC </t>
+  </si>
+  <si>
+    <t xml:space="preserve">274011</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MONTURA 1 x 1  EPOXI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">276083</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NIPLE 1  x 100 cm EPOXI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">278049</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NIPLE 1  x  20 cm BRONCE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">280083</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NIPLE 2   x   8 cm PPN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">312001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">REDUCCION HM 3/4 x 1/2 CROMO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">332013</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BOTON LATERAL CAPEA CROMO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">332085</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MANIJA CUADRADA BRONCE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">332093</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MECANISMO ANDINO BRONCE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">332213</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BOTON CONCAVO DEALER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">342053</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PICO LAVATORIO COMPLETO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">342059</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PICO PEIRANO MESADA ANTIGUO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">354003</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SIFON DOBLE  GOMA RAO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">376005</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TAPA FRANKLIN INTERNA COMPLETA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">390019</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TERMOTANQUE POPULI G.E </t>
+  </si>
+  <si>
+    <t xml:space="preserve">408011</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UNIDAD MAGNETICA 309 ORBIS </t>
+  </si>
+  <si>
+    <t xml:space="preserve">424057</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SOMBRERO H DE ZINC 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">438187</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TAPON M 1/2 EPOXI DEMA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">438250</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CUPLA RED 3/4 X 1/2  GALV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">449163</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VIVA PLUS LAVATORIO PICO </t>
+  </si>
+  <si>
+    <t xml:space="preserve">449165</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VIVA PLUS BANERA </t>
+  </si>
+  <si>
+    <t xml:space="preserve">450307</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LLAVIN ESFERICO HH 1/2 </t>
   </si>
 </sst>
 </file>
@@ -297,17 +423,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C38"/>
+  <dimension ref="A1:C49"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E31" activeCellId="0" sqref="E31"/>
+      <selection pane="topLeft" activeCell="B50" activeCellId="0" sqref="B50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="32.27"/>
   </cols>
@@ -331,7 +457,7 @@
         <v>4</v>
       </c>
       <c r="C2" s="2" t="n">
-        <v>179.1</v>
+        <v>106.08</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -342,7 +468,7 @@
         <v>6</v>
       </c>
       <c r="C3" s="2" t="n">
-        <v>306.06</v>
+        <v>109.26</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -353,7 +479,7 @@
         <v>8</v>
       </c>
       <c r="C4" s="2" t="n">
-        <v>110.51</v>
+        <v>1233.29</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -364,7 +490,7 @@
         <v>10</v>
       </c>
       <c r="C5" s="2" t="n">
-        <v>104.27</v>
+        <v>219.34</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -375,7 +501,7 @@
         <v>12</v>
       </c>
       <c r="C6" s="2" t="n">
-        <v>186.37</v>
+        <v>186.15</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -386,7 +512,7 @@
         <v>14</v>
       </c>
       <c r="C7" s="2" t="n">
-        <v>187.76</v>
+        <v>507.75</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -397,7 +523,7 @@
         <v>16</v>
       </c>
       <c r="C8" s="2" t="n">
-        <v>132.05</v>
+        <v>75.56</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -408,7 +534,7 @@
         <v>18</v>
       </c>
       <c r="C9" s="2" t="n">
-        <v>233.83</v>
+        <v>1123.32</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -419,7 +545,7 @@
         <v>20</v>
       </c>
       <c r="C10" s="2" t="n">
-        <v>374.82</v>
+        <v>85.76</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -430,7 +556,7 @@
         <v>22</v>
       </c>
       <c r="C11" s="2" t="n">
-        <v>129.21</v>
+        <v>1099.19</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -441,7 +567,7 @@
         <v>24</v>
       </c>
       <c r="C12" s="2" t="n">
-        <v>220.67</v>
+        <v>118.48</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -452,7 +578,7 @@
         <v>26</v>
       </c>
       <c r="C13" s="2" t="n">
-        <v>346.07</v>
+        <v>180.88</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -463,7 +589,7 @@
         <v>28</v>
       </c>
       <c r="C14" s="2" t="n">
-        <v>186.72</v>
+        <v>20.16</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -474,7 +600,7 @@
         <v>30</v>
       </c>
       <c r="C15" s="2" t="n">
-        <v>193.99</v>
+        <v>1410.75</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -485,7 +611,7 @@
         <v>32</v>
       </c>
       <c r="C16" s="2" t="n">
-        <v>324.24</v>
+        <v>1606.76</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -496,7 +622,7 @@
         <v>34</v>
       </c>
       <c r="C17" s="2" t="n">
-        <v>180.83</v>
+        <v>1032.94</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -507,7 +633,7 @@
         <v>36</v>
       </c>
       <c r="C18" s="2" t="n">
-        <v>272.97</v>
+        <v>429.07</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -518,7 +644,7 @@
         <v>38</v>
       </c>
       <c r="C19" s="2" t="n">
-        <v>454.5</v>
+        <v>583.47</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -529,7 +655,7 @@
         <v>40</v>
       </c>
       <c r="C20" s="2" t="n">
-        <v>118.47</v>
+        <v>328.44</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -540,7 +666,7 @@
         <v>42</v>
       </c>
       <c r="C21" s="2" t="n">
-        <v>204.38</v>
+        <v>1117.82</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -551,7 +677,7 @@
         <v>44</v>
       </c>
       <c r="C22" s="2" t="n">
-        <v>99.77</v>
+        <v>15.38</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -562,7 +688,7 @@
         <v>46</v>
       </c>
       <c r="C23" s="2" t="n">
-        <v>124.88</v>
+        <v>12407.01</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -573,7 +699,7 @@
         <v>48</v>
       </c>
       <c r="C24" s="2" t="n">
-        <v>216.51</v>
+        <v>19487.3</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -584,7 +710,7 @@
         <v>50</v>
       </c>
       <c r="C25" s="2" t="n">
-        <v>404.61</v>
+        <v>29705.54</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -595,7 +721,7 @@
         <v>52</v>
       </c>
       <c r="C26" s="2" t="n">
-        <v>132.68</v>
+        <v>2196.74</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -606,7 +732,7 @@
         <v>54</v>
       </c>
       <c r="C27" s="2" t="n">
-        <v>196.42</v>
+        <v>7152.11</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -617,48 +743,244 @@
         <v>56</v>
       </c>
       <c r="C28" s="2" t="n">
-        <v>278.86</v>
+        <v>416.55</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B29" s="1"/>
-      <c r="C29" s="2"/>
+      <c r="A29" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C29" s="2" t="n">
+        <v>1270.48</v>
+      </c>
     </row>
     <row r="30" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B30" s="1"/>
-      <c r="C30" s="2"/>
+      <c r="A30" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C30" s="2" t="n">
+        <v>2514.69</v>
+      </c>
     </row>
     <row r="31" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B31" s="1"/>
-      <c r="C31" s="2"/>
+      <c r="A31" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C31" s="2" t="n">
+        <v>2328.18</v>
+      </c>
     </row>
     <row r="32" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B32" s="1"/>
-      <c r="C32" s="2"/>
+      <c r="A32" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C32" s="2" t="n">
+        <v>267.78</v>
+      </c>
     </row>
     <row r="33" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B33" s="1"/>
-      <c r="C33" s="2"/>
+      <c r="A33" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C33" s="2" t="n">
+        <v>685.71</v>
+      </c>
     </row>
     <row r="34" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C34" s="2"/>
+      <c r="A34" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C34" s="2" t="n">
+        <v>352.8</v>
+      </c>
     </row>
     <row r="35" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C35" s="2"/>
+      <c r="A35" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C35" s="2" t="n">
+        <v>1180.43</v>
+      </c>
     </row>
     <row r="36" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C36" s="2"/>
+      <c r="A36" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C36" s="2" t="n">
+        <v>2288.55</v>
+      </c>
     </row>
     <row r="37" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C37" s="2"/>
+      <c r="A37" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C37" s="2" t="n">
+        <v>357.54</v>
+      </c>
     </row>
     <row r="38" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C38" s="2"/>
+      <c r="A38" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C38" s="2" t="n">
+        <v>4041.17</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C39" s="2" t="n">
+        <v>3017.5</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C40" s="2" t="n">
+        <v>1310.46</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C41" s="2" t="n">
+        <v>440.54</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C42" s="2" t="n">
+        <v>44437.54</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C43" s="2" t="n">
+        <v>1666.53</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C44" s="2" t="n">
+        <v>1596.84</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C45" s="2" t="n">
+        <v>108.05</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C46" s="2" t="n">
+        <v>197.37</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C47" s="2" t="n">
+        <v>7500.73</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C48" s="2" t="n">
+        <v>10471.71</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C49" s="2" t="n">
+        <v>628.71</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>

</xml_diff>